<commit_message>
Added Abstract, FFT subchapter, fixed errors found by ***
</commit_message>
<xml_diff>
--- a/docs/NN time efficiency.xlsx
+++ b/docs/NN time efficiency.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="21">
   <si>
     <t>INPUTS</t>
   </si>
@@ -58,9 +58,6 @@
   </si>
   <si>
     <t>20s</t>
-  </si>
-  <si>
-    <t>None - only preprocessor ran; returned hardcoded zeros as probabilities</t>
   </si>
   <si>
     <t>None - only preprocessor and postprocessor ran; returned hardcoded zeros as probabilities</t>
@@ -265,49 +262,49 @@
   </cellStyleXfs>
   <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -607,7 +604,7 @@
   <dimension ref="A1:D16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G14" sqref="G14"/>
+      <selection activeCell="F14" sqref="F14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -617,172 +614,185 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="13" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="13" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" s="13" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="6" t="s">
+      <c r="D1" s="14" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="2" spans="1:4" ht="15.75" thickBot="1">
-      <c r="A2" s="2"/>
-      <c r="B2" s="2"/>
-      <c r="C2" s="2"/>
-      <c r="D2" s="7"/>
+      <c r="A2" s="7"/>
+      <c r="B2" s="7"/>
+      <c r="C2" s="7"/>
+      <c r="D2" s="15"/>
     </row>
     <row r="3" spans="1:4">
-      <c r="A3" s="4" t="s">
+      <c r="A3" s="9" t="s">
         <v>11</v>
       </c>
-      <c r="B3" s="4" t="s">
+      <c r="B3" s="9" t="s">
         <v>5</v>
       </c>
-      <c r="C3" s="12" t="s">
+      <c r="C3" s="10" t="s">
         <v>12</v>
       </c>
-      <c r="D3" s="8" t="s">
+      <c r="D3" s="12" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="4" spans="1:4">
-      <c r="A4" s="5"/>
-      <c r="B4" s="5"/>
-      <c r="C4" s="14"/>
-      <c r="D4" s="9"/>
+      <c r="A4" s="2"/>
+      <c r="B4" s="2"/>
+      <c r="C4" s="11"/>
+      <c r="D4" s="1"/>
     </row>
     <row r="5" spans="1:4">
-      <c r="A5" s="5" t="s">
+      <c r="A5" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="B5" s="5" t="s">
+      <c r="B5" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="C5" s="15" t="s">
+      <c r="C5" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4">
+      <c r="A6" s="2"/>
+      <c r="B6" s="2"/>
+      <c r="C6" s="6"/>
+      <c r="D6" s="1"/>
+    </row>
+    <row r="7" spans="1:4">
+      <c r="A7" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C7" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="D7" s="1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4">
+      <c r="A8" s="2"/>
+      <c r="B8" s="2"/>
+      <c r="C8" s="3"/>
+      <c r="D8" s="1"/>
+    </row>
+    <row r="9" spans="1:4" ht="15" customHeight="1">
+      <c r="A9" s="2">
+        <v>257</v>
+      </c>
+      <c r="B9" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C9" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="D9" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="D5" s="9" t="s">
+    </row>
+    <row r="10" spans="1:4">
+      <c r="A10" s="2"/>
+      <c r="B10" s="2"/>
+      <c r="C10" s="6"/>
+      <c r="D10" s="1"/>
+    </row>
+    <row r="11" spans="1:4">
+      <c r="A11" s="2">
+        <v>257</v>
+      </c>
+      <c r="B11" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C11" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="D11" s="1" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4">
+      <c r="A12" s="2"/>
+      <c r="B12" s="2"/>
+      <c r="C12" s="4"/>
+      <c r="D12" s="1"/>
+    </row>
+    <row r="13" spans="1:4" ht="15" customHeight="1">
+      <c r="A13" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="B13" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="C13" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="D13" s="1" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="6" spans="1:4">
-      <c r="A6" s="5"/>
-      <c r="B6" s="5"/>
-      <c r="C6" s="13"/>
-      <c r="D6" s="9"/>
-    </row>
-    <row r="7" spans="1:4">
-      <c r="A7" s="5" t="s">
-        <v>7</v>
-      </c>
-      <c r="B7" s="5" t="s">
-        <v>5</v>
-      </c>
-      <c r="C7" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="D7" s="9" t="s">
+    <row r="14" spans="1:4">
+      <c r="A14" s="2"/>
+      <c r="B14" s="2"/>
+      <c r="C14" s="6"/>
+      <c r="D14" s="1"/>
+    </row>
+    <row r="15" spans="1:4">
+      <c r="A15" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="B15" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="C15" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="D15" s="1" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="8" spans="1:4">
-      <c r="A8" s="5"/>
-      <c r="B8" s="5"/>
-      <c r="C8" s="11"/>
-      <c r="D8" s="9"/>
-    </row>
-    <row r="9" spans="1:4">
-      <c r="A9" s="5">
-        <v>257</v>
-      </c>
-      <c r="B9" s="5" t="s">
-        <v>5</v>
-      </c>
-      <c r="C9" s="15" t="s">
-        <v>14</v>
-      </c>
-      <c r="D9" s="9" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4">
-      <c r="A10" s="5"/>
-      <c r="B10" s="5"/>
-      <c r="C10" s="13"/>
-      <c r="D10" s="9"/>
-    </row>
-    <row r="11" spans="1:4">
-      <c r="A11" s="5">
-        <v>257</v>
-      </c>
-      <c r="B11" s="5" t="s">
-        <v>5</v>
-      </c>
-      <c r="C11" s="11" t="s">
-        <v>4</v>
-      </c>
-      <c r="D11" s="9" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4">
-      <c r="A12" s="5"/>
-      <c r="B12" s="5"/>
-      <c r="C12" s="3"/>
-      <c r="D12" s="9"/>
-    </row>
-    <row r="13" spans="1:4">
-      <c r="A13" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="B13" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="C13" s="15" t="s">
-        <v>14</v>
-      </c>
-      <c r="D13" s="9" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4">
-      <c r="A14" s="5"/>
-      <c r="B14" s="5"/>
-      <c r="C14" s="13"/>
-      <c r="D14" s="9"/>
-    </row>
-    <row r="15" spans="1:4">
-      <c r="A15" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="B15" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="C15" s="5" t="s">
-        <v>3</v>
-      </c>
-      <c r="D15" s="9" t="s">
-        <v>18</v>
-      </c>
-    </row>
     <row r="16" spans="1:4" ht="15.75" thickBot="1">
-      <c r="A16" s="2"/>
-      <c r="B16" s="2"/>
-      <c r="C16" s="2"/>
-      <c r="D16" s="10"/>
+      <c r="A16" s="7"/>
+      <c r="B16" s="7"/>
+      <c r="C16" s="7"/>
+      <c r="D16" s="8"/>
     </row>
   </sheetData>
   <mergeCells count="32">
-    <mergeCell ref="D9:D10"/>
-    <mergeCell ref="A11:A12"/>
-    <mergeCell ref="B11:B12"/>
-    <mergeCell ref="C11:C12"/>
-    <mergeCell ref="D11:D12"/>
+    <mergeCell ref="A3:A4"/>
+    <mergeCell ref="B3:B4"/>
+    <mergeCell ref="C3:C4"/>
+    <mergeCell ref="D3:D4"/>
+    <mergeCell ref="A1:A2"/>
+    <mergeCell ref="B1:B2"/>
+    <mergeCell ref="C1:C2"/>
+    <mergeCell ref="D1:D2"/>
+    <mergeCell ref="D5:D6"/>
+    <mergeCell ref="D7:D8"/>
+    <mergeCell ref="A5:A6"/>
+    <mergeCell ref="B5:B6"/>
+    <mergeCell ref="C5:C6"/>
+    <mergeCell ref="A7:A8"/>
+    <mergeCell ref="B7:B8"/>
+    <mergeCell ref="C7:C8"/>
+    <mergeCell ref="B9:B10"/>
+    <mergeCell ref="C9:C10"/>
     <mergeCell ref="A13:A14"/>
     <mergeCell ref="B13:B14"/>
     <mergeCell ref="C13:C14"/>
@@ -791,27 +801,15 @@
     <mergeCell ref="B15:B16"/>
     <mergeCell ref="C15:C16"/>
     <mergeCell ref="D15:D16"/>
+    <mergeCell ref="D9:D10"/>
+    <mergeCell ref="A11:A12"/>
+    <mergeCell ref="B11:B12"/>
+    <mergeCell ref="C11:C12"/>
+    <mergeCell ref="D11:D12"/>
     <mergeCell ref="A9:A10"/>
-    <mergeCell ref="A7:A8"/>
-    <mergeCell ref="B7:B8"/>
-    <mergeCell ref="C7:C8"/>
-    <mergeCell ref="B9:B10"/>
-    <mergeCell ref="C9:C10"/>
-    <mergeCell ref="D5:D6"/>
-    <mergeCell ref="D7:D8"/>
-    <mergeCell ref="A5:A6"/>
-    <mergeCell ref="B5:B6"/>
-    <mergeCell ref="C5:C6"/>
-    <mergeCell ref="A3:A4"/>
-    <mergeCell ref="B3:B4"/>
-    <mergeCell ref="C3:C4"/>
-    <mergeCell ref="D3:D4"/>
-    <mergeCell ref="A1:A2"/>
-    <mergeCell ref="B1:B2"/>
-    <mergeCell ref="C1:C2"/>
-    <mergeCell ref="D1:D2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 

</xml_diff>